<commit_message>
Significant documentation changes, with a problem
I documented all the stuff in 'inst/' in the hope of making it easier to
use the examples in the docstrings as well as in the hopes of making
this package a bit more accessible.  Unfortunately, my various
invocations of system.file(package="hpgltools") in 01_hpgltools.r
cause the installation to fail now, unless one uses
'--no-staged-install'.  For the moment, I will leave this as-is, but
will check in with Theresa if it works for her.
</commit_message>
<xml_diff>
--- a/inst/share/pa_samples.xlsx
+++ b/inst/share/pa_samples.xlsx
@@ -142,7 +142,7 @@
     <t xml:space="preserve">Large</t>
   </si>
   <si>
-    <t xml:space="preserve">wild_type</t>
+    <t xml:space="preserve">delta_orn</t>
   </si>
   <si>
     <t xml:space="preserve">Stationary</t>
@@ -272,6 +272,9 @@
     <t xml:space="preserve">Day 6</t>
   </si>
   <si>
+    <t xml:space="preserve">wild_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">L_wt_st</t>
   </si>
   <si>
@@ -330,9 +333,6 @@
   </si>
   <si>
     <t xml:space="preserve">L / EX / Day 2 / Δ.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delta_orn</t>
   </si>
   <si>
     <t xml:space="preserve">Exponential</t>
@@ -471,7 +471,7 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
-    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
@@ -699,12 +699,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -770,17 +770,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA14" activeCellId="0" sqref="AA14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.97"/>
@@ -804,7 +804,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="16.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="23.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,7 +889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -979,7 +978,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>48</v>
       </c>
@@ -1171,13 +1170,13 @@
         <v>30</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H5" s="16" t="n">
         <v>42899</v>
@@ -1189,7 +1188,7 @@
         <v>34</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L5" s="15" t="n">
         <v>4</v>
@@ -1228,19 +1227,19 @@
         <v>11.0352941176471</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X5" s="18" t="s">
         <v>38</v>
       </c>
       <c r="Y5" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z5" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA5" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB5" s="15" t="s">
         <v>54</v>
@@ -1248,10 +1247,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>56</v>
@@ -1260,13 +1259,13 @@
         <v>30</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H6" s="20" t="n">
         <v>42899</v>
@@ -1278,7 +1277,7 @@
         <v>34</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L6" s="19" t="n">
         <v>4</v>
@@ -1317,30 +1316,30 @@
         <v>14.7153846153846</v>
       </c>
       <c r="W6" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X6" s="22" t="s">
         <v>38</v>
       </c>
       <c r="Y6" s="22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z6" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB6" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>56</v>
@@ -1349,13 +1348,13 @@
         <v>30</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H7" s="24" t="n">
         <v>42899</v>
@@ -1367,7 +1366,7 @@
         <v>34</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L7" s="23" t="n">
         <v>4</v>
@@ -1406,30 +1405,30 @@
         <v>16.0916666666667</v>
       </c>
       <c r="W7" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="X7" s="26" t="s">
         <v>38</v>
       </c>
       <c r="Y7" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z7" s="23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AB7" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>29</v>
@@ -1438,7 +1437,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>78</v>
@@ -1510,7 +1509,7 @@
         <v>84</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,7 +1526,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>78</v>
@@ -1616,7 +1615,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>78</v>
@@ -1705,7 +1704,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>78</v>
@@ -1790,7 +1789,7 @@
         <v>30</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>78</v>
@@ -1879,7 +1878,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>78</v>
@@ -1966,7 +1965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1976,10 +1975,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">

</xml_diff>